<commit_message>
Modified files, corrected features values
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +116,8 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -187,9 +185,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,7 +472,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +523,7 @@
       <c r="M2" s="5">
         <v>6</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="13">
         <v>9</v>
       </c>
     </row>
@@ -567,7 +566,7 @@
       <c r="M3">
         <v>12</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="14">
         <v>18</v>
       </c>
       <c r="O3">
@@ -618,7 +617,7 @@
       <c r="M4">
         <v>18</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="14">
         <v>19</v>
       </c>
       <c r="O4">
@@ -734,18 +733,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -761,7 +760,7 @@
       </c>
       <c r="I11" s="1">
         <f>SUM(B11:H11)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J11">
         <f>2/4.75</f>
@@ -773,11 +772,11 @@
       <c r="L11">
         <v>11</v>
       </c>
-      <c r="M11" s="11">
-        <v>8</v>
-      </c>
-      <c r="N11" s="11">
-        <v>11</v>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
       </c>
       <c r="O11">
         <v>9</v>
@@ -793,7 +792,7 @@
       </c>
       <c r="S11">
         <f>SUM(L11:R11)</f>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="T11">
         <f>71/121</f>
@@ -862,7 +861,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -872,11 +871,11 @@
       </c>
       <c r="C13">
         <f t="shared" ref="C13:H13" si="1">C11/C12</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -896,22 +895,16 @@
       </c>
       <c r="I13" s="1">
         <f>I11/I12</f>
-        <v>0.10526315789473684</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
-      </c>
-      <c r="M13">
-        <v>7</v>
-      </c>
-      <c r="N13">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.55" x14ac:dyDescent="0.35">
       <c r="I14">
         <f>_xlfn.STDEV.S(B13:H13)</f>
-        <v>0.14433756729740643</v>
+        <v>0.20331251519761109</v>
       </c>
       <c r="J14" t="s">
         <v>5</v>
@@ -992,11 +985,11 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1018,7 +1011,7 @@
       </c>
       <c r="J19" s="1">
         <f>SUM(B19:I19)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19">
         <f>1/6</f>
@@ -1027,14 +1020,14 @@
       <c r="L19" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="7">
-        <v>10</v>
-      </c>
-      <c r="N19" s="7">
-        <v>12</v>
-      </c>
-      <c r="O19" s="7">
-        <v>13</v>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <v>17</v>
       </c>
       <c r="P19">
         <v>14</v>
@@ -1053,7 +1046,7 @@
       </c>
       <c r="U19">
         <f>SUM(M19:T19)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="V19">
         <f>102/119</f>
@@ -1074,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -1090,7 +1083,7 @@
       </c>
       <c r="J20" s="1">
         <f>SUM(B20:I20)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K20">
         <f>24/4</f>
@@ -1134,15 +1127,15 @@
       </c>
       <c r="B21">
         <f>B19/B20</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:I21" si="2">B19/B20</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
@@ -1166,28 +1159,16 @@
       </c>
       <c r="J21" s="1">
         <f>J19/J20</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.12</v>
       </c>
       <c r="K21" t="s">
         <v>4</v>
       </c>
-      <c r="M21">
-        <v>9</v>
-      </c>
-      <c r="N21">
-        <v>11</v>
-      </c>
-      <c r="O21">
-        <v>17</v>
-      </c>
     </row>
     <row r="22" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="E22">
-        <v>5</v>
-      </c>
       <c r="J22">
         <f>_xlfn.STDEV.S(B21:I21)</f>
-        <v>0.17677669529663689</v>
+        <v>0.18600595228571123</v>
       </c>
       <c r="K22" t="s">
         <v>5</v>
@@ -1875,28 +1856,28 @@
       <c r="J22" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="12"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
@@ -1906,12 +1887,12 @@
         <f>62+62</f>
         <v>124</v>
       </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
     </row>
     <row r="26" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F26" t="s">

</xml_diff>

<commit_message>
Overall_spatial_chan_Avg segmented w.r.t marker_block
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BNBO" sheetId="1" r:id="rId1"/>
@@ -14,16 +14,11 @@
     <sheet name="JF" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="21">
   <si>
     <t>Ses 3</t>
   </si>
@@ -82,14 +77,17 @@
     <t>Total Catch</t>
   </si>
   <si>
-    <t>7 (discard)</t>
+    <t>Removed Ses 5, Block 3 - because subject was given more instructions in the middle of this block</t>
+  </si>
+  <si>
+    <t>7 (discard because subject started feeliong pain)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +114,135 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,18 +251,197 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -163,11 +467,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -177,7 +629,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -187,20 +638,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -461,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +1078,7 @@
       <c r="M3">
         <v>12</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="12">
         <v>18</v>
       </c>
       <c r="O3">
@@ -617,7 +1129,7 @@
       <c r="M4">
         <v>18</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>19</v>
       </c>
       <c r="O4">
@@ -737,30 +1249,30 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>1</v>
+      </c>
+      <c r="H11" s="17">
         <v>0</v>
       </c>
       <c r="I11" s="1">
         <f>SUM(B11:H11)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <f>2/4.75</f>
@@ -769,30 +1281,30 @@
       <c r="K11" t="s">
         <v>14</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="18">
         <v>11</v>
       </c>
-      <c r="M11">
-        <v>7</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="18">
+        <v>8</v>
+      </c>
+      <c r="N11" s="18">
+        <v>11</v>
+      </c>
+      <c r="O11" s="18">
+        <v>9</v>
+      </c>
+      <c r="P11" s="18">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="18">
         <v>10</v>
       </c>
-      <c r="O11">
-        <v>9</v>
-      </c>
-      <c r="P11">
-        <v>13</v>
-      </c>
-      <c r="Q11">
-        <v>10</v>
-      </c>
-      <c r="R11">
+      <c r="R11" s="18">
         <v>9</v>
       </c>
       <c r="S11">
         <f>SUM(L11:R11)</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T11">
         <f>71/121</f>
@@ -803,25 +1315,25 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
+      <c r="B12" s="17">
+        <v>3</v>
+      </c>
+      <c r="C12" s="17">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17">
+        <v>2</v>
+      </c>
+      <c r="E12" s="17">
+        <v>3</v>
+      </c>
+      <c r="F12" s="17">
+        <v>2</v>
+      </c>
+      <c r="G12" s="17">
+        <v>4</v>
+      </c>
+      <c r="H12" s="17">
         <v>2</v>
       </c>
       <c r="I12" s="1">
@@ -835,25 +1347,25 @@
       <c r="K12" t="s">
         <v>11</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="18">
         <v>17</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="18">
         <v>17</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="18">
         <v>18</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="18">
         <v>17</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="18">
         <v>18</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="18">
         <v>16</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="18">
         <v>18</v>
       </c>
       <c r="S12">
@@ -871,11 +1383,11 @@
       </c>
       <c r="C13">
         <f t="shared" ref="C13:H13" si="1">C11/C12</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -895,16 +1407,16 @@
       </c>
       <c r="I13" s="1">
         <f>I11/I12</f>
-        <v>0.21052631578947367</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="J13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I14">
         <f>_xlfn.STDEV.S(B13:H13)</f>
-        <v>0.20331251519761109</v>
+        <v>0.14433756729740643</v>
       </c>
       <c r="J14" t="s">
         <v>5</v>
@@ -924,7 +1436,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -985,33 +1497,33 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="7">
-        <v>1</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
+      <c r="B19" s="20">
+        <v>0</v>
+      </c>
+      <c r="C19" s="20">
+        <v>0</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0</v>
+      </c>
+      <c r="F19" s="20">
+        <v>0</v>
+      </c>
+      <c r="G19" s="20">
+        <v>1</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0</v>
+      </c>
+      <c r="I19" s="20">
         <v>0</v>
       </c>
       <c r="J19" s="1">
         <f>SUM(B19:I19)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <f>1/6</f>
@@ -1020,33 +1532,33 @@
       <c r="L19" t="s">
         <v>10</v>
       </c>
-      <c r="M19">
-        <v>9</v>
-      </c>
-      <c r="N19">
+      <c r="M19" s="19">
+        <v>10</v>
+      </c>
+      <c r="N19" s="19">
+        <v>12</v>
+      </c>
+      <c r="O19" s="19">
+        <v>17</v>
+      </c>
+      <c r="P19" s="19">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>16</v>
+      </c>
+      <c r="R19" s="19">
         <v>11</v>
       </c>
-      <c r="O19">
-        <v>17</v>
-      </c>
-      <c r="P19">
-        <v>14</v>
-      </c>
-      <c r="Q19">
-        <v>16</v>
-      </c>
-      <c r="R19">
-        <v>11</v>
-      </c>
-      <c r="S19">
+      <c r="S19" s="19">
         <v>13</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="19">
         <v>13</v>
       </c>
       <c r="U19">
         <f>SUM(M19:T19)</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="V19">
         <f>102/119</f>
@@ -1057,28 +1569,28 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="B20" s="20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="20">
         <v>5</v>
       </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20">
+      <c r="F20" s="20">
+        <v>2</v>
+      </c>
+      <c r="G20" s="20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="20">
+        <v>3</v>
+      </c>
+      <c r="I20" s="20">
         <v>4</v>
       </c>
       <c r="J20" s="1">
@@ -1092,28 +1604,28 @@
       <c r="L20" t="s">
         <v>11</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="19">
         <v>16</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="19">
         <v>16</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="19">
         <v>19</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="19">
         <v>15</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="19">
         <v>18</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="19">
         <v>18</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="19">
         <v>17</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="19">
         <v>16</v>
       </c>
       <c r="U20">
@@ -1127,15 +1639,15 @@
       </c>
       <c r="B21">
         <f>B19/B20</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:I21" si="2">B19/B20</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
@@ -1159,7 +1671,7 @@
       </c>
       <c r="J21" s="1">
         <f>J19/J20</f>
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="K21" t="s">
         <v>4</v>
@@ -1168,7 +1680,7 @@
     <row r="22" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="J22">
         <f>_xlfn.STDEV.S(B21:I21)</f>
-        <v>0.18600595228571123</v>
+        <v>0.17677669529663689</v>
       </c>
       <c r="K22" t="s">
         <v>5</v>
@@ -1228,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,13 +1886,13 @@
       <c r="M10" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="13">
         <v>3</v>
       </c>
       <c r="O10" s="5">
         <v>4</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="13">
         <v>5</v>
       </c>
       <c r="Q10" s="5">
@@ -1399,32 +1911,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="B11" s="36">
+        <v>0</v>
+      </c>
+      <c r="C11" s="36">
+        <v>0</v>
+      </c>
+      <c r="D11" s="36">
+        <v>1</v>
+      </c>
+      <c r="E11" s="36">
+        <v>1</v>
+      </c>
+      <c r="F11" s="36">
+        <v>1</v>
+      </c>
+      <c r="G11" s="36">
+        <v>0</v>
+      </c>
+      <c r="H11" s="36">
+        <v>0</v>
+      </c>
+      <c r="I11" s="36">
         <v>2</v>
       </c>
       <c r="J11" s="1">
@@ -1438,33 +1950,33 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="12">
         <v>9</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="36">
         <v>5</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="12">
+        <v>12</v>
+      </c>
+      <c r="Q11" s="36">
+        <v>10</v>
+      </c>
+      <c r="R11" s="36">
+        <v>10</v>
+      </c>
+      <c r="S11" s="36">
+        <v>11</v>
+      </c>
+      <c r="T11" s="36">
         <v>5</v>
       </c>
-      <c r="Q11">
-        <v>10</v>
-      </c>
-      <c r="R11">
-        <v>8</v>
-      </c>
-      <c r="S11">
-        <v>11</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-      <c r="U11">
+      <c r="U11" s="36">
         <v>9</v>
       </c>
       <c r="V11">
         <f>SUM(N11:U11)</f>
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="W11">
         <f>62/138</f>
@@ -1475,28 +1987,28 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="B12" s="36">
+        <v>3</v>
+      </c>
+      <c r="C12" s="36">
+        <v>2</v>
+      </c>
+      <c r="D12" s="36">
+        <v>1</v>
+      </c>
+      <c r="E12" s="36">
+        <v>3</v>
+      </c>
+      <c r="F12" s="36">
+        <v>1</v>
+      </c>
+      <c r="G12" s="36">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="36">
+        <v>3</v>
+      </c>
+      <c r="I12" s="36">
         <v>4</v>
       </c>
       <c r="J12" s="1">
@@ -1510,28 +2022,28 @@
       <c r="M12" t="s">
         <v>3</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="12">
         <v>17</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="36">
         <v>18</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="12">
         <v>19</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="36">
         <v>17</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="36">
         <v>19</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="36">
         <v>15</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="36">
         <v>17</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="36">
         <v>16</v>
       </c>
       <c r="V12">
@@ -1582,33 +2094,17 @@
       <c r="K13" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="7">
-        <v>8</v>
-      </c>
-      <c r="O13" s="7">
-        <v>5</v>
-      </c>
-      <c r="P13" s="7">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>10</v>
-      </c>
-      <c r="R13" s="7">
-        <v>10</v>
-      </c>
-      <c r="S13" s="7">
-        <v>10</v>
-      </c>
-      <c r="T13" s="7">
-        <v>5</v>
-      </c>
-      <c r="U13" s="7">
-        <v>9</v>
-      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
       <c r="V13">
         <f>SUM(N13:U13)</f>
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.25">
@@ -1664,10 +2160,10 @@
       <c r="N18" s="5">
         <v>4</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="13">
         <v>5</v>
       </c>
-      <c r="P18" s="5">
+      <c r="P18" s="13">
         <v>6</v>
       </c>
       <c r="Q18" s="5">
@@ -1687,19 +2183,19 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
+      <c r="D19" s="23">
+        <v>0</v>
+      </c>
+      <c r="E19" s="23">
+        <v>2</v>
+      </c>
+      <c r="F19" s="23">
+        <v>2</v>
+      </c>
+      <c r="G19" s="23">
+        <v>0</v>
+      </c>
+      <c r="H19" s="23">
         <v>1</v>
       </c>
       <c r="I19" s="1">
@@ -1713,19 +2209,19 @@
       <c r="M19" t="s">
         <v>10</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="22">
         <v>10</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="12">
         <v>13</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="12">
         <v>12</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="22">
         <v>14</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="22">
         <v>13</v>
       </c>
       <c r="S19">
@@ -1747,19 +2243,19 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
+      <c r="D20" s="23">
+        <v>2</v>
+      </c>
+      <c r="E20" s="23">
+        <v>3</v>
+      </c>
+      <c r="F20" s="23">
+        <v>4</v>
+      </c>
+      <c r="G20" s="23">
+        <v>2</v>
+      </c>
+      <c r="H20" s="23">
         <v>4</v>
       </c>
       <c r="I20" s="1">
@@ -1773,19 +2269,19 @@
       <c r="M20" t="s">
         <v>11</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="22">
         <v>18</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="12">
         <v>17</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="12">
         <v>16</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="22">
         <v>18</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="22">
         <v>16</v>
       </c>
       <c r="S20">
@@ -1832,21 +2328,11 @@
       <c r="J21" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="7">
-        <v>10</v>
-      </c>
-      <c r="O21" s="7">
-        <v>12</v>
-      </c>
-      <c r="P21" s="7">
-        <v>12</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>14</v>
-      </c>
-      <c r="R21" s="7">
-        <v>13</v>
-      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I22" t="e">
@@ -1856,28 +2342,28 @@
       <c r="J22" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
@@ -1887,12 +2373,12 @@
         <f>62+62</f>
         <v>124</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
     </row>
     <row r="26" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
@@ -1905,7 +2391,7 @@
       <c r="I26">
         <v>0.55600000000000005</v>
       </c>
-      <c r="O26" s="9"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
@@ -1927,10 +2413,11 @@
       <c r="I29">
         <v>0.27</v>
       </c>
-      <c r="O29" s="8"/>
+      <c r="O29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1938,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O28" sqref="O27:O28"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1970,37 +2457,37 @@
       <c r="D2" s="5">
         <v>6</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="15">
         <v>7</v>
       </c>
       <c r="F2" s="1"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
-        <v>4</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="J2" s="13">
+        <v>4</v>
+      </c>
+      <c r="K2" s="13">
         <v>5</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="13">
         <v>6</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="M2" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="31">
+        <v>2</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+      <c r="D3" s="31">
         <v>0</v>
       </c>
       <c r="E3">
@@ -2017,13 +2504,13 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <v>8</v>
       </c>
-      <c r="K3">
-        <v>13</v>
-      </c>
-      <c r="L3">
+      <c r="K3" s="12">
+        <v>14</v>
+      </c>
+      <c r="L3" s="12">
         <v>12</v>
       </c>
       <c r="M3">
@@ -2031,24 +2518,24 @@
       </c>
       <c r="N3">
         <f>SUM(J3:M3)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O3">
         <f>45/70</f>
         <v>0.6428571428571429</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="31">
+        <v>2</v>
+      </c>
+      <c r="C4" s="31">
+        <v>1</v>
+      </c>
+      <c r="D4" s="31">
         <v>2</v>
       </c>
       <c r="E4">
@@ -2065,13 +2552,13 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="12">
         <v>18</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="12">
         <v>19</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="12">
         <v>18</v>
       </c>
       <c r="M4">
@@ -2082,7 +2569,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2109,17 +2596,11 @@
       <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="7">
-        <v>7</v>
-      </c>
-      <c r="K5" s="7">
-        <v>14</v>
-      </c>
-      <c r="L5" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F6">
         <f>_xlfn.STDEV.S(B5:E5)*100</f>
         <v>47.871355387816905</v>
@@ -2177,10 +2658,10 @@
       <c r="M10" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="5">
-        <v>1</v>
-      </c>
-      <c r="O10" s="5">
+      <c r="N10" s="13">
+        <v>1</v>
+      </c>
+      <c r="O10" s="13">
         <v>2</v>
       </c>
       <c r="P10" s="5">
@@ -2192,17 +2673,17 @@
       <c r="R10" s="5">
         <v>6</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="13">
         <v>7</v>
       </c>
-      <c r="T10" s="5">
+      <c r="T10" s="13">
         <v>8</v>
       </c>
-      <c r="U10" s="5">
+      <c r="U10" s="13">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2224,13 +2705,13 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
+      <c r="H11" s="32">
+        <v>3</v>
+      </c>
+      <c r="I11" s="32">
+        <v>1</v>
+      </c>
+      <c r="J11" s="32">
         <v>3</v>
       </c>
       <c r="K11" s="1">
@@ -2244,10 +2725,10 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="12">
         <v>10</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="12">
         <v>10</v>
       </c>
       <c r="P11">
@@ -2259,25 +2740,25 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="S11" s="7">
-        <v>7</v>
-      </c>
-      <c r="T11">
+      <c r="S11" s="12">
+        <v>9</v>
+      </c>
+      <c r="T11" s="12">
         <v>14</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="12">
         <v>15</v>
       </c>
       <c r="V11">
         <f>SUM(N11:U11)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="W11">
         <f>55/124</f>
         <v>0.44354838709677419</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2299,29 +2780,29 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="32">
         <v>5</v>
       </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
+      <c r="I12" s="32">
+        <v>2</v>
+      </c>
+      <c r="J12" s="32">
         <v>4</v>
       </c>
       <c r="K12" s="1">
         <f>SUM(B12:J12)</f>
         <v>21</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <v>5</v>
       </c>
       <c r="M12" t="s">
         <v>11</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="12">
         <v>17</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="12">
         <v>17</v>
       </c>
       <c r="P12">
@@ -2333,13 +2814,13 @@
       <c r="R12">
         <v>19</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="12">
         <v>15</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="12">
         <v>18</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="12">
         <v>16</v>
       </c>
       <c r="V12">
@@ -2347,7 +2828,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2394,32 +2875,16 @@
       <c r="L13" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="7">
-        <v>8</v>
-      </c>
-      <c r="O13" s="7">
-        <v>10</v>
-      </c>
-      <c r="P13" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>5</v>
-      </c>
-      <c r="R13" s="7">
-        <v>16</v>
-      </c>
-      <c r="S13" s="7">
-        <v>7</v>
-      </c>
-      <c r="T13" s="7">
-        <v>14</v>
-      </c>
-      <c r="U13" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="K14" t="e">
         <f>_xlfn.STDEV.S(B13:J13)*100</f>
         <v>#DIV/0!</v>
@@ -2442,7 +2907,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2483,22 +2948,22 @@
       <c r="P18" s="5">
         <v>3</v>
       </c>
-      <c r="Q18" s="5">
-        <v>4</v>
-      </c>
-      <c r="R18" s="5">
+      <c r="Q18" s="16">
+        <v>4</v>
+      </c>
+      <c r="R18" s="16">
         <v>5</v>
       </c>
       <c r="S18" s="5">
         <v>7</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="16">
         <v>8</v>
       </c>
       <c r="U18" s="5">
         <v>9</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="16">
         <v>10</v>
       </c>
       <c r="W18" s="5">
@@ -2509,36 +2974,36 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="J19">
+      <c r="B19" s="34">
+        <v>2</v>
+      </c>
+      <c r="C19" s="34">
+        <v>0</v>
+      </c>
+      <c r="D19" s="34">
+        <v>3</v>
+      </c>
+      <c r="E19" s="34">
+        <v>1</v>
+      </c>
+      <c r="F19" s="34">
+        <v>2</v>
+      </c>
+      <c r="G19" s="34">
+        <v>0</v>
+      </c>
+      <c r="H19" s="34">
+        <v>1</v>
+      </c>
+      <c r="I19" s="34">
+        <v>2</v>
+      </c>
+      <c r="J19" s="34">
         <v>2</v>
       </c>
       <c r="K19" s="1">
         <f>SUM(B19:J19)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L19">
         <f>11/5.25</f>
@@ -2547,36 +3012,36 @@
       <c r="N19" t="s">
         <v>10</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="33">
         <v>11</v>
       </c>
-      <c r="P19">
-        <v>2</v>
-      </c>
-      <c r="Q19">
+      <c r="P19" s="33">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="21">
         <v>10</v>
       </c>
-      <c r="R19">
-        <v>5</v>
-      </c>
-      <c r="S19">
+      <c r="R19" s="21">
+        <v>13</v>
+      </c>
+      <c r="S19" s="33">
         <v>7</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="21">
         <v>9</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="33">
         <v>10</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="21">
         <v>12</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="33">
         <v>12</v>
       </c>
       <c r="X19">
         <f>SUM(O19:W19)</f>
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="Y19">
         <f>78/158</f>
@@ -2587,31 +3052,31 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="7">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <v>3</v>
-      </c>
-      <c r="J20">
+      <c r="B20" s="34">
+        <v>3</v>
+      </c>
+      <c r="C20" s="34">
+        <v>1</v>
+      </c>
+      <c r="D20" s="34">
+        <v>3</v>
+      </c>
+      <c r="E20" s="34">
+        <v>1</v>
+      </c>
+      <c r="F20" s="34">
+        <v>4</v>
+      </c>
+      <c r="G20" s="34">
+        <v>3</v>
+      </c>
+      <c r="H20" s="34">
+        <v>2</v>
+      </c>
+      <c r="I20" s="34">
+        <v>3</v>
+      </c>
+      <c r="J20" s="34">
         <v>2</v>
       </c>
       <c r="K20" s="1">
@@ -2625,31 +3090,31 @@
       <c r="N20" t="s">
         <v>11</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="33">
         <v>17</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="33">
         <v>19</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="21">
         <v>17</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="21">
         <v>19</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="33">
         <v>16</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="21">
         <v>17</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="33">
         <v>18</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="21">
         <v>17</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="33">
         <v>18</v>
       </c>
       <c r="X20">
@@ -2663,7 +3128,7 @@
       </c>
       <c r="B21">
         <f>B19/B20</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:J21" si="2">C19/C20</f>
@@ -2671,7 +3136,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
@@ -2699,43 +3164,25 @@
       </c>
       <c r="K21" s="1">
         <f>K19/K20</f>
-        <v>0.5</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
       </c>
-      <c r="O21" s="7">
-        <v>11</v>
-      </c>
-      <c r="P21" s="7">
-        <v>11</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>10</v>
-      </c>
-      <c r="R21" s="7">
-        <v>12</v>
-      </c>
-      <c r="S21" s="7">
-        <v>6</v>
-      </c>
-      <c r="T21" s="7">
-        <v>9</v>
-      </c>
-      <c r="U21" s="7">
-        <v>10</v>
-      </c>
-      <c r="V21" s="7">
-        <v>11</v>
-      </c>
-      <c r="W21" s="7">
-        <v>12</v>
-      </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="K22">
         <f>_xlfn.STDEV.S(B21:J21)*100</f>
-        <v>36.746545987008219</v>
+        <v>39.185377721294131</v>
       </c>
       <c r="L22" t="s">
         <v>9</v>
@@ -2791,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,73 +3295,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="C3" s="25">
+        <v>0</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25">
         <v>0</v>
       </c>
       <c r="G3" s="1">
         <f>SUM(B3:F3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="24">
         <v>13</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="24">
         <v>10</v>
       </c>
-      <c r="M3">
-        <v>15</v>
-      </c>
-      <c r="N3">
+      <c r="M3" s="24">
+        <v>16</v>
+      </c>
+      <c r="N3" s="24">
         <v>13</v>
       </c>
       <c r="O3">
         <f>SUM(K3:N3)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P3">
         <f>37/71</f>
         <v>0.52112676056338025</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="C4" s="25">
+        <v>3</v>
+      </c>
+      <c r="D4" s="25">
+        <v>2</v>
+      </c>
+      <c r="E4" s="25">
+        <v>1</v>
+      </c>
+      <c r="F4" s="25">
         <v>3</v>
       </c>
       <c r="G4" s="1">
@@ -2928,16 +3375,16 @@
       <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="24">
         <v>17</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="24">
         <v>18</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="24">
         <v>19</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="24">
         <v>17</v>
       </c>
       <c r="O4">
@@ -2980,9 +3427,7 @@
       <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="7">
-        <v>15</v>
-      </c>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G6" t="e">
@@ -3064,66 +3509,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="B11" s="27">
+        <v>0</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27">
+        <v>0</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27">
         <v>0</v>
       </c>
       <c r="J11" s="1">
         <f>SUM(B11:I11)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>0</v>
       </c>
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="26">
         <v>14</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="26">
         <v>8</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="26">
         <v>12</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="26">
         <v>16</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="26">
         <v>16</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="26">
         <v>15</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="26">
         <v>16</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11" s="26">
         <v>16</v>
       </c>
       <c r="V11">
@@ -3135,66 +3580,66 @@
         <v>0.77857142857142858</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
+      <c r="B12" s="27">
+        <v>2</v>
+      </c>
+      <c r="C12" s="27">
+        <v>2</v>
+      </c>
+      <c r="D12" s="27">
+        <v>3</v>
+      </c>
+      <c r="E12" s="27">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27">
+        <v>3</v>
+      </c>
+      <c r="G12" s="27">
+        <v>3</v>
+      </c>
+      <c r="H12" s="27">
+        <v>4</v>
+      </c>
+      <c r="I12" s="27">
         <v>2</v>
       </c>
       <c r="J12" s="1">
         <f>SUM(B12:I12)</f>
         <v>20</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>5</v>
       </c>
       <c r="M12" t="s">
         <v>11</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="26">
         <v>18</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="26">
         <v>18</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="26">
         <v>17</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="26">
         <v>19</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="26">
         <v>17</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="26">
         <v>17</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="26">
         <v>16</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="26">
         <v>18</v>
       </c>
       <c r="V12">
@@ -3202,7 +3647,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>B11/B12</f>
         <v>0</v>
@@ -3243,7 +3688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J14">
         <f>_xlfn.STDEV.S(B13:I13)</f>
         <v>0</v>
@@ -3252,7 +3697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3266,11 +3711,11 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="15">
         <v>3</v>
       </c>
       <c r="C18" s="5">
@@ -3302,184 +3747,175 @@
         <v>1</v>
       </c>
       <c r="O18" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P18" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R18" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S18" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T18" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U18" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="V18" s="5">
-        <v>10</v>
-      </c>
-      <c r="W18" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
+      <c r="C19" s="30">
+        <v>1</v>
+      </c>
+      <c r="D19" s="30">
+        <v>0</v>
+      </c>
+      <c r="E19" s="30">
+        <v>0</v>
+      </c>
+      <c r="F19" s="30">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30">
+        <v>0</v>
+      </c>
+      <c r="I19" s="30">
+        <v>0</v>
+      </c>
+      <c r="J19" s="30">
         <v>2</v>
       </c>
       <c r="K19" s="1">
         <f>SUM(B19:J19)</f>
         <v>3</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="9">
         <v>0.75</v>
       </c>
       <c r="N19" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="7">
-        <v>9</v>
-      </c>
-      <c r="P19" s="7">
+      <c r="O19" s="28">
         <v>8</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="P19" s="28">
         <v>11</v>
       </c>
-      <c r="R19" s="7">
+      <c r="Q19" s="28">
         <v>8</v>
       </c>
-      <c r="S19" s="7">
+      <c r="R19" s="28">
         <v>7</v>
       </c>
-      <c r="T19" s="7">
+      <c r="S19" s="28">
         <v>15</v>
       </c>
-      <c r="U19" s="7">
+      <c r="T19" s="28">
         <v>14</v>
       </c>
-      <c r="V19" s="7">
+      <c r="U19" s="28">
         <v>11</v>
       </c>
-      <c r="W19" s="7">
-        <v>13</v>
+      <c r="V19" s="28">
+        <v>14</v>
+      </c>
+      <c r="W19">
+        <f>SUM(O19:V19)</f>
+        <v>88</v>
       </c>
       <c r="X19">
-        <f>SUM(O19:W19)</f>
-        <v>96</v>
-      </c>
-      <c r="Y19">
         <f>85/164</f>
         <v>0.51829268292682928</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
+      <c r="C20" s="30">
+        <v>3</v>
+      </c>
+      <c r="D20" s="30">
+        <v>1</v>
+      </c>
+      <c r="E20" s="30">
+        <v>2</v>
+      </c>
+      <c r="F20" s="30">
+        <v>1</v>
+      </c>
+      <c r="G20" s="30">
+        <v>1</v>
+      </c>
+      <c r="H20" s="30">
+        <v>1</v>
+      </c>
+      <c r="I20" s="30">
+        <v>1</v>
+      </c>
+      <c r="J20" s="30">
         <v>3</v>
       </c>
       <c r="K20" s="1">
         <f>SUM(B20:J20)</f>
         <v>16</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>4</v>
       </c>
       <c r="N20" t="s">
         <v>11</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="29">
         <v>17</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="29">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>18</v>
+      </c>
+      <c r="R20" s="29">
+        <v>19</v>
+      </c>
+      <c r="S20" s="29">
+        <v>19</v>
+      </c>
+      <c r="T20" s="29">
+        <v>19</v>
+      </c>
+      <c r="U20" s="29">
+        <v>19</v>
+      </c>
+      <c r="V20" s="29">
         <v>17</v>
       </c>
-      <c r="Q20">
-        <v>19</v>
-      </c>
-      <c r="R20">
-        <v>18</v>
-      </c>
-      <c r="S20">
-        <v>19</v>
-      </c>
-      <c r="T20">
-        <v>19</v>
-      </c>
-      <c r="U20">
-        <v>19</v>
-      </c>
-      <c r="V20">
-        <v>19</v>
-      </c>
       <c r="W20">
-        <v>17</v>
-      </c>
-      <c r="X20">
-        <f>SUM(O20:W20)</f>
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+        <f>SUM(O20:V20)</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" ref="B21:J21" si="2">B19/B20</f>
         <v>0</v>
@@ -3524,7 +3960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K22">
         <f>_xlfn.STDEV.S(B21:J21)*100</f>
         <v>23.570226039551585</v>
@@ -3532,11 +3968,14 @@
       <c r="L22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>15</v>
       </c>
@@ -3545,7 +3984,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>16</v>
       </c>
@@ -3558,10 +3997,10 @@
       </c>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>17</v>
       </c>
@@ -3570,7 +4009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>18</v>
       </c>
@@ -3584,6 +4023,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3591,8 +4031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3843,7 +4283,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3900,66 +4340,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
+      <c r="B19" s="36">
+        <v>0</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0</v>
+      </c>
+      <c r="E19" s="36">
+        <v>0</v>
+      </c>
+      <c r="F19" s="36">
+        <v>0</v>
+      </c>
+      <c r="G19" s="36">
+        <v>0</v>
+      </c>
+      <c r="H19" s="36">
+        <v>0</v>
+      </c>
+      <c r="I19" s="36">
         <v>0</v>
       </c>
       <c r="J19" s="1">
         <f>SUM(B19:I19)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>0</v>
       </c>
       <c r="M19" t="s">
         <v>10</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="35">
         <v>14</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="35">
         <v>17</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="35">
         <v>17</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="35">
         <v>15</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="35">
         <v>17</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="35">
         <v>13</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="35">
         <v>12</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="35">
         <v>18</v>
       </c>
       <c r="V19">
@@ -3967,66 +4407,66 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20">
+      <c r="B20" s="36">
+        <v>4</v>
+      </c>
+      <c r="C20" s="36">
+        <v>2</v>
+      </c>
+      <c r="D20" s="36">
+        <v>3</v>
+      </c>
+      <c r="E20" s="36">
+        <v>1</v>
+      </c>
+      <c r="F20" s="36">
+        <v>2</v>
+      </c>
+      <c r="G20" s="36">
+        <v>4</v>
+      </c>
+      <c r="H20" s="36">
+        <v>2</v>
+      </c>
+      <c r="I20" s="36">
         <v>2</v>
       </c>
       <c r="J20" s="1">
         <f>SUM(B20:I20)</f>
         <v>20</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>5</v>
       </c>
       <c r="M20" t="s">
         <v>11</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="35">
         <v>16</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="35">
         <v>18</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="35">
         <v>17</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="35">
         <v>19</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="35">
         <v>18</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="35">
         <v>16</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="35">
         <v>18</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="35">
         <v>18</v>
       </c>
       <c r="V20">
@@ -4034,7 +4474,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B21">
         <f>B19/B20</f>
         <v>0</v>

</xml_diff>

<commit_message>
Most recent update after resolving all bugs :)
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BNBO" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="25">
   <si>
     <t>Ses 3</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>7 (discard because subject started feeliong pain)</t>
+  </si>
+  <si>
+    <t>For 6 trials, Intent detected but EEG_GO, EMG_GO decisions were 0</t>
+  </si>
+  <si>
+    <t>waitng for Ted's reply</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>TR</t>
   </si>
 </sst>
 </file>
@@ -242,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,19 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,15 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -663,6 +661,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -983,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +1047,7 @@
       <c r="M2" s="5">
         <v>6</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="11">
         <v>9</v>
       </c>
     </row>
@@ -1078,7 +1090,7 @@
       <c r="M3">
         <v>12</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="10">
         <v>18</v>
       </c>
       <c r="O3">
@@ -1129,7 +1141,7 @@
       <c r="M4">
         <v>18</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="10">
         <v>19</v>
       </c>
       <c r="O4">
@@ -1171,6 +1183,15 @@
       </c>
       <c r="I5" t="s">
         <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1249,25 +1270,25 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17">
-        <v>1</v>
-      </c>
-      <c r="C11" s="17">
-        <v>0</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <v>0</v>
-      </c>
-      <c r="F11" s="17">
-        <v>0</v>
-      </c>
-      <c r="G11" s="17">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+      <c r="H11" s="14">
         <v>0</v>
       </c>
       <c r="I11" s="1">
@@ -1281,25 +1302,25 @@
       <c r="K11" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="15">
         <v>11</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="15">
         <v>8</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="15">
         <v>11</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="15">
         <v>9</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="15">
         <v>13</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="15">
         <v>10</v>
       </c>
-      <c r="R11" s="18">
+      <c r="R11" s="15">
         <v>9</v>
       </c>
       <c r="S11">
@@ -1315,25 +1336,25 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17">
-        <v>3</v>
-      </c>
-      <c r="C12" s="17">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17">
-        <v>2</v>
-      </c>
-      <c r="E12" s="17">
-        <v>3</v>
-      </c>
-      <c r="F12" s="17">
-        <v>2</v>
-      </c>
-      <c r="G12" s="17">
-        <v>4</v>
-      </c>
-      <c r="H12" s="17">
+      <c r="B12" s="14">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3</v>
+      </c>
+      <c r="F12" s="14">
+        <v>2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4</v>
+      </c>
+      <c r="H12" s="14">
         <v>2</v>
       </c>
       <c r="I12" s="1">
@@ -1347,25 +1368,25 @@
       <c r="K12" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="15">
         <v>17</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="15">
         <v>17</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="15">
         <v>18</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="15">
         <v>17</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="15">
         <v>18</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="15">
         <v>16</v>
       </c>
-      <c r="R12" s="18">
+      <c r="R12" s="15">
         <v>18</v>
       </c>
       <c r="S12">
@@ -1411,6 +1432,27 @@
       </c>
       <c r="J13" t="s">
         <v>4</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -1497,28 +1539,28 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="20">
-        <v>0</v>
-      </c>
-      <c r="C19" s="20">
-        <v>0</v>
-      </c>
-      <c r="D19" s="20">
-        <v>0</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0</v>
-      </c>
-      <c r="G19" s="20">
-        <v>1</v>
-      </c>
-      <c r="H19" s="20">
-        <v>0</v>
-      </c>
-      <c r="I19" s="20">
+      <c r="B19" s="17">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>0</v>
+      </c>
+      <c r="I19" s="17">
         <v>0</v>
       </c>
       <c r="J19" s="1">
@@ -1532,28 +1574,28 @@
       <c r="L19" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="16">
         <v>10</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="16">
         <v>12</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="16">
         <v>17</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="16">
         <v>14</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="Q19" s="16">
         <v>16</v>
       </c>
-      <c r="R19" s="19">
+      <c r="R19" s="16">
         <v>11</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="16">
         <v>13</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="16">
         <v>13</v>
       </c>
       <c r="U19">
@@ -1569,28 +1611,28 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="20">
-        <v>4</v>
-      </c>
-      <c r="C20" s="20">
-        <v>4</v>
-      </c>
-      <c r="D20" s="20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="20">
+      <c r="B20" s="17">
+        <v>4</v>
+      </c>
+      <c r="C20" s="17">
+        <v>4</v>
+      </c>
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="17">
         <v>5</v>
       </c>
-      <c r="F20" s="20">
-        <v>2</v>
-      </c>
-      <c r="G20" s="20">
-        <v>2</v>
-      </c>
-      <c r="H20" s="20">
-        <v>3</v>
-      </c>
-      <c r="I20" s="20">
+      <c r="F20" s="17">
+        <v>2</v>
+      </c>
+      <c r="G20" s="17">
+        <v>2</v>
+      </c>
+      <c r="H20" s="17">
+        <v>3</v>
+      </c>
+      <c r="I20" s="17">
         <v>4</v>
       </c>
       <c r="J20" s="1">
@@ -1604,28 +1646,28 @@
       <c r="L20" t="s">
         <v>11</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="16">
         <v>16</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="16">
         <v>16</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="16">
         <v>19</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="16">
         <v>15</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="Q20" s="16">
         <v>18</v>
       </c>
-      <c r="R20" s="19">
+      <c r="R20" s="16">
         <v>18</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S20" s="16">
         <v>17</v>
       </c>
-      <c r="T20" s="19">
+      <c r="T20" s="16">
         <v>16</v>
       </c>
       <c r="U20">
@@ -1676,6 +1718,31 @@
       <c r="K21" t="s">
         <v>4</v>
       </c>
+      <c r="M21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="U21" s="32"/>
     </row>
     <row r="22" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="J22">
@@ -1740,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1886,13 +1953,13 @@
       <c r="M10" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="13">
-        <v>3</v>
-      </c>
-      <c r="O10" s="5">
-        <v>4</v>
-      </c>
-      <c r="P10" s="13">
+      <c r="N10" s="11">
+        <v>3</v>
+      </c>
+      <c r="O10" s="11">
+        <v>4</v>
+      </c>
+      <c r="P10" s="11">
         <v>5</v>
       </c>
       <c r="Q10" s="5">
@@ -1915,28 +1982,28 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="36">
-        <v>0</v>
-      </c>
-      <c r="C11" s="36">
-        <v>0</v>
-      </c>
-      <c r="D11" s="36">
-        <v>1</v>
-      </c>
-      <c r="E11" s="36">
-        <v>1</v>
-      </c>
-      <c r="F11" s="36">
-        <v>1</v>
-      </c>
-      <c r="G11" s="36">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36">
-        <v>0</v>
-      </c>
-      <c r="I11" s="36">
+      <c r="B11" s="32">
+        <v>0</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <v>1</v>
+      </c>
+      <c r="E11" s="32">
+        <v>1</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="32">
         <v>2</v>
       </c>
       <c r="J11" s="1">
@@ -1950,28 +2017,28 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="10">
         <v>9</v>
       </c>
-      <c r="O11" s="36">
+      <c r="O11" s="10">
         <v>5</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="10">
         <v>12</v>
       </c>
-      <c r="Q11" s="36">
+      <c r="Q11" s="32">
         <v>10</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="32">
         <v>10</v>
       </c>
-      <c r="S11" s="36">
+      <c r="S11" s="32">
         <v>11</v>
       </c>
-      <c r="T11" s="36">
+      <c r="T11" s="32">
         <v>5</v>
       </c>
-      <c r="U11" s="36">
+      <c r="U11" s="32">
         <v>9</v>
       </c>
       <c r="V11">
@@ -1987,28 +2054,28 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="36">
-        <v>3</v>
-      </c>
-      <c r="C12" s="36">
-        <v>2</v>
-      </c>
-      <c r="D12" s="36">
-        <v>1</v>
-      </c>
-      <c r="E12" s="36">
-        <v>3</v>
-      </c>
-      <c r="F12" s="36">
-        <v>1</v>
-      </c>
-      <c r="G12" s="36">
+      <c r="B12" s="32">
+        <v>3</v>
+      </c>
+      <c r="C12" s="32">
+        <v>2</v>
+      </c>
+      <c r="D12" s="32">
+        <v>1</v>
+      </c>
+      <c r="E12" s="32">
+        <v>3</v>
+      </c>
+      <c r="F12" s="32">
+        <v>1</v>
+      </c>
+      <c r="G12" s="32">
         <v>5</v>
       </c>
-      <c r="H12" s="36">
-        <v>3</v>
-      </c>
-      <c r="I12" s="36">
+      <c r="H12" s="32">
+        <v>3</v>
+      </c>
+      <c r="I12" s="32">
         <v>4</v>
       </c>
       <c r="J12" s="1">
@@ -2022,28 +2089,28 @@
       <c r="M12" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="10">
         <v>17</v>
       </c>
-      <c r="O12" s="36">
+      <c r="O12" s="10">
         <v>18</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="10">
         <v>19</v>
       </c>
-      <c r="Q12" s="36">
+      <c r="Q12" s="32">
         <v>17</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="32">
         <v>19</v>
       </c>
-      <c r="S12" s="36">
+      <c r="S12" s="32">
         <v>15</v>
       </c>
-      <c r="T12" s="36">
+      <c r="T12" s="32">
         <v>17</v>
       </c>
-      <c r="U12" s="36">
+      <c r="U12" s="32">
         <v>16</v>
       </c>
       <c r="V12">
@@ -2157,13 +2224,13 @@
       <c r="M18" t="s">
         <v>1</v>
       </c>
-      <c r="N18" s="5">
-        <v>4</v>
-      </c>
-      <c r="O18" s="13">
+      <c r="N18" s="11">
+        <v>4</v>
+      </c>
+      <c r="O18" s="11">
         <v>5</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="11">
         <v>6</v>
       </c>
       <c r="Q18" s="5">
@@ -2183,19 +2250,19 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" s="23">
-        <v>0</v>
-      </c>
-      <c r="E19" s="23">
-        <v>2</v>
-      </c>
-      <c r="F19" s="23">
-        <v>2</v>
-      </c>
-      <c r="G19" s="23">
-        <v>0</v>
-      </c>
-      <c r="H19" s="23">
+      <c r="D19" s="19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="19">
+        <v>2</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="19">
         <v>1</v>
       </c>
       <c r="I19" s="1">
@@ -2209,19 +2276,19 @@
       <c r="M19" t="s">
         <v>10</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="10">
         <v>10</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="10">
         <v>13</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="10">
         <v>12</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="18">
         <v>14</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="18">
         <v>13</v>
       </c>
       <c r="S19">
@@ -2243,19 +2310,19 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20" s="23">
-        <v>2</v>
-      </c>
-      <c r="E20" s="23">
-        <v>3</v>
-      </c>
-      <c r="F20" s="23">
-        <v>4</v>
-      </c>
-      <c r="G20" s="23">
-        <v>2</v>
-      </c>
-      <c r="H20" s="23">
+      <c r="D20" s="19">
+        <v>2</v>
+      </c>
+      <c r="E20" s="19">
+        <v>3</v>
+      </c>
+      <c r="F20" s="19">
+        <v>4</v>
+      </c>
+      <c r="G20" s="19">
+        <v>2</v>
+      </c>
+      <c r="H20" s="19">
         <v>4</v>
       </c>
       <c r="I20" s="1">
@@ -2269,19 +2336,19 @@
       <c r="M20" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="22">
+      <c r="N20" s="10">
         <v>18</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="10">
         <v>17</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="10">
         <v>16</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="18">
         <v>18</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="18">
         <v>16</v>
       </c>
       <c r="S20">
@@ -2425,14 +2492,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="13" max="13" width="9.77734375" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.25">
@@ -2457,23 +2525,23 @@
       <c r="D2" s="5">
         <v>6</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <v>7</v>
       </c>
       <c r="F2" s="1"/>
       <c r="I2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="13">
-        <v>4</v>
-      </c>
-      <c r="K2" s="13">
+      <c r="J2" s="11">
+        <v>4</v>
+      </c>
+      <c r="K2" s="11">
         <v>5</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <v>6</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2481,13 +2549,13 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="31">
-        <v>2</v>
-      </c>
-      <c r="C3" s="31">
-        <v>1</v>
-      </c>
-      <c r="D3" s="31">
+      <c r="B3" s="27">
+        <v>2</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27">
         <v>0</v>
       </c>
       <c r="E3">
@@ -2504,13 +2572,13 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="10">
         <v>8</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="10">
         <v>14</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="10">
         <v>12</v>
       </c>
       <c r="M3">
@@ -2529,13 +2597,13 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="31">
-        <v>2</v>
-      </c>
-      <c r="C4" s="31">
-        <v>1</v>
-      </c>
-      <c r="D4" s="31">
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="27">
         <v>2</v>
       </c>
       <c r="E4">
@@ -2552,13 +2620,13 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>18</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="10">
         <v>19</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>18</v>
       </c>
       <c r="M4">
@@ -2658,28 +2726,28 @@
       <c r="M10" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="13">
-        <v>1</v>
-      </c>
-      <c r="O10" s="13">
+      <c r="N10" s="33">
+        <v>1</v>
+      </c>
+      <c r="O10" s="11">
         <v>2</v>
       </c>
       <c r="P10" s="5">
         <v>3</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="33">
         <v>5</v>
       </c>
       <c r="R10" s="5">
         <v>6</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="11">
         <v>7</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="11">
         <v>8</v>
       </c>
-      <c r="U10" s="13">
+      <c r="U10" s="11">
         <v>9</v>
       </c>
     </row>
@@ -2705,13 +2773,13 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" s="32">
-        <v>3</v>
-      </c>
-      <c r="I11" s="32">
-        <v>1</v>
-      </c>
-      <c r="J11" s="32">
+      <c r="H11" s="28">
+        <v>3</v>
+      </c>
+      <c r="I11" s="28">
+        <v>1</v>
+      </c>
+      <c r="J11" s="28">
         <v>3</v>
       </c>
       <c r="K11" s="1">
@@ -2725,33 +2793,33 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="10">
         <v>10</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="10">
         <v>10</v>
       </c>
-      <c r="P11">
-        <v>2</v>
-      </c>
-      <c r="Q11">
-        <v>3</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11" s="12">
+      <c r="P11" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>5</v>
+      </c>
+      <c r="R11" s="10">
+        <v>16</v>
+      </c>
+      <c r="S11" s="10">
         <v>9</v>
       </c>
-      <c r="T11" s="12">
+      <c r="T11" s="10">
         <v>14</v>
       </c>
-      <c r="U11" s="12">
+      <c r="U11" s="10">
         <v>15</v>
       </c>
       <c r="V11">
         <f>SUM(N11:U11)</f>
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="W11">
         <f>55/124</f>
@@ -2780,13 +2848,13 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="28">
         <v>5</v>
       </c>
-      <c r="I12" s="32">
-        <v>2</v>
-      </c>
-      <c r="J12" s="32">
+      <c r="I12" s="28">
+        <v>2</v>
+      </c>
+      <c r="J12" s="28">
         <v>4</v>
       </c>
       <c r="K12" s="1">
@@ -2799,28 +2867,28 @@
       <c r="M12" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="10">
         <v>17</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="10">
         <v>17</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="10">
         <v>18</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="10">
         <v>19</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="10">
         <v>19</v>
       </c>
-      <c r="S12" s="12">
+      <c r="S12" s="10">
         <v>15</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="10">
         <v>18</v>
       </c>
-      <c r="U12" s="12">
+      <c r="U12" s="10">
         <v>16</v>
       </c>
       <c r="V12">
@@ -2828,7 +2896,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2875,10 +2943,14 @@
       <c r="L13" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="10"/>
+      <c r="N13" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="Q13" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -2945,25 +3017,25 @@
       <c r="O18" s="5">
         <v>2</v>
       </c>
-      <c r="P18" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="16">
-        <v>4</v>
-      </c>
-      <c r="R18" s="16">
+      <c r="P18" s="11">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>4</v>
+      </c>
+      <c r="R18" s="11">
         <v>5</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="11">
         <v>7</v>
       </c>
-      <c r="T18" s="16">
+      <c r="T18" s="11">
         <v>8</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="11">
         <v>9</v>
       </c>
-      <c r="V18" s="16">
+      <c r="V18" s="11">
         <v>10</v>
       </c>
       <c r="W18" s="5">
@@ -2974,31 +3046,31 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="34">
-        <v>2</v>
-      </c>
-      <c r="C19" s="34">
-        <v>0</v>
-      </c>
-      <c r="D19" s="34">
-        <v>3</v>
-      </c>
-      <c r="E19" s="34">
-        <v>1</v>
-      </c>
-      <c r="F19" s="34">
-        <v>2</v>
-      </c>
-      <c r="G19" s="34">
-        <v>0</v>
-      </c>
-      <c r="H19" s="34">
-        <v>1</v>
-      </c>
-      <c r="I19" s="34">
-        <v>2</v>
-      </c>
-      <c r="J19" s="34">
+      <c r="B19" s="30">
+        <v>2</v>
+      </c>
+      <c r="C19" s="30">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30">
+        <v>3</v>
+      </c>
+      <c r="E19" s="30">
+        <v>1</v>
+      </c>
+      <c r="F19" s="30">
+        <v>2</v>
+      </c>
+      <c r="G19" s="30">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30">
+        <v>1</v>
+      </c>
+      <c r="I19" s="30">
+        <v>2</v>
+      </c>
+      <c r="J19" s="30">
         <v>2</v>
       </c>
       <c r="K19" s="1">
@@ -3012,31 +3084,31 @@
       <c r="N19" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="33">
+      <c r="O19" s="29">
         <v>11</v>
       </c>
-      <c r="P19" s="33">
+      <c r="P19" s="10">
         <v>11</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="10">
         <v>10</v>
       </c>
-      <c r="R19" s="21">
+      <c r="R19" s="10">
         <v>13</v>
       </c>
-      <c r="S19" s="33">
+      <c r="S19" s="10">
         <v>7</v>
       </c>
-      <c r="T19" s="21">
+      <c r="T19" s="10">
         <v>9</v>
       </c>
-      <c r="U19" s="33">
+      <c r="U19" s="10">
         <v>10</v>
       </c>
-      <c r="V19" s="21">
+      <c r="V19" s="10">
         <v>12</v>
       </c>
-      <c r="W19" s="33">
+      <c r="W19" s="29">
         <v>12</v>
       </c>
       <c r="X19">
@@ -3052,31 +3124,31 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="34">
-        <v>3</v>
-      </c>
-      <c r="C20" s="34">
-        <v>1</v>
-      </c>
-      <c r="D20" s="34">
-        <v>3</v>
-      </c>
-      <c r="E20" s="34">
-        <v>1</v>
-      </c>
-      <c r="F20" s="34">
-        <v>4</v>
-      </c>
-      <c r="G20" s="34">
-        <v>3</v>
-      </c>
-      <c r="H20" s="34">
-        <v>2</v>
-      </c>
-      <c r="I20" s="34">
-        <v>3</v>
-      </c>
-      <c r="J20" s="34">
+      <c r="B20" s="30">
+        <v>3</v>
+      </c>
+      <c r="C20" s="30">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <v>3</v>
+      </c>
+      <c r="E20" s="30">
+        <v>1</v>
+      </c>
+      <c r="F20" s="30">
+        <v>4</v>
+      </c>
+      <c r="G20" s="30">
+        <v>3</v>
+      </c>
+      <c r="H20" s="30">
+        <v>2</v>
+      </c>
+      <c r="I20" s="30">
+        <v>3</v>
+      </c>
+      <c r="J20" s="30">
         <v>2</v>
       </c>
       <c r="K20" s="1">
@@ -3090,31 +3162,31 @@
       <c r="N20" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="33">
+      <c r="O20" s="29">
         <v>17</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="10">
         <v>19</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="10">
         <v>17</v>
       </c>
-      <c r="R20" s="21">
+      <c r="R20" s="10">
         <v>19</v>
       </c>
-      <c r="S20" s="33">
+      <c r="S20" s="10">
         <v>16</v>
       </c>
-      <c r="T20" s="21">
+      <c r="T20" s="10">
         <v>17</v>
       </c>
-      <c r="U20" s="33">
+      <c r="U20" s="10">
         <v>18</v>
       </c>
-      <c r="V20" s="21">
+      <c r="V20" s="10">
         <v>17</v>
       </c>
-      <c r="W20" s="33">
+      <c r="W20" s="29">
         <v>18</v>
       </c>
       <c r="X20">
@@ -3169,15 +3241,15 @@
       <c r="L21" t="s">
         <v>4</v>
       </c>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="K22">
@@ -3240,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3302,16 +3374,16 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="25">
-        <v>0</v>
-      </c>
-      <c r="D3" s="25">
-        <v>0</v>
-      </c>
-      <c r="E3" s="25">
-        <v>0</v>
-      </c>
-      <c r="F3" s="25">
+      <c r="C3" s="21">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21">
         <v>0</v>
       </c>
       <c r="G3" s="1">
@@ -3324,16 +3396,16 @@
       <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="20">
         <v>13</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="20">
         <v>10</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="20">
         <v>16</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="20">
         <v>13</v>
       </c>
       <c r="O3">
@@ -3352,16 +3424,16 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="25">
-        <v>3</v>
-      </c>
-      <c r="D4" s="25">
-        <v>2</v>
-      </c>
-      <c r="E4" s="25">
-        <v>1</v>
-      </c>
-      <c r="F4" s="25">
+      <c r="C4" s="21">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21">
+        <v>2</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
         <v>3</v>
       </c>
       <c r="G4" s="1">
@@ -3375,16 +3447,16 @@
       <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="20">
         <v>17</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="20">
         <v>18</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="20">
         <v>19</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="20">
         <v>17</v>
       </c>
       <c r="O4">
@@ -3427,7 +3499,18 @@
       <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="K5" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G6" t="e">
@@ -3513,28 +3596,28 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="27">
-        <v>0</v>
-      </c>
-      <c r="C11" s="27">
-        <v>0</v>
-      </c>
-      <c r="D11" s="27">
-        <v>0</v>
-      </c>
-      <c r="E11" s="27">
-        <v>0</v>
-      </c>
-      <c r="F11" s="27">
-        <v>0</v>
-      </c>
-      <c r="G11" s="27">
-        <v>0</v>
-      </c>
-      <c r="H11" s="27">
-        <v>0</v>
-      </c>
-      <c r="I11" s="27">
+      <c r="B11" s="23">
+        <v>0</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0</v>
+      </c>
+      <c r="F11" s="23">
+        <v>0</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0</v>
+      </c>
+      <c r="I11" s="23">
         <v>0</v>
       </c>
       <c r="J11" s="1">
@@ -3547,28 +3630,28 @@
       <c r="M11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="26">
+      <c r="N11" s="22">
         <v>14</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="22">
         <v>8</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="22">
         <v>12</v>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="22">
         <v>16</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="22">
         <v>16</v>
       </c>
-      <c r="S11" s="26">
+      <c r="S11" s="22">
         <v>15</v>
       </c>
-      <c r="T11" s="26">
+      <c r="T11" s="22">
         <v>16</v>
       </c>
-      <c r="U11" s="26">
+      <c r="U11" s="22">
         <v>16</v>
       </c>
       <c r="V11">
@@ -3584,28 +3667,28 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="27">
-        <v>2</v>
-      </c>
-      <c r="C12" s="27">
-        <v>2</v>
-      </c>
-      <c r="D12" s="27">
-        <v>3</v>
-      </c>
-      <c r="E12" s="27">
-        <v>1</v>
-      </c>
-      <c r="F12" s="27">
-        <v>3</v>
-      </c>
-      <c r="G12" s="27">
-        <v>3</v>
-      </c>
-      <c r="H12" s="27">
-        <v>4</v>
-      </c>
-      <c r="I12" s="27">
+      <c r="B12" s="23">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23">
+        <v>3</v>
+      </c>
+      <c r="E12" s="23">
+        <v>1</v>
+      </c>
+      <c r="F12" s="23">
+        <v>3</v>
+      </c>
+      <c r="G12" s="23">
+        <v>3</v>
+      </c>
+      <c r="H12" s="23">
+        <v>4</v>
+      </c>
+      <c r="I12" s="23">
         <v>2</v>
       </c>
       <c r="J12" s="1">
@@ -3618,28 +3701,28 @@
       <c r="M12" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="26">
+      <c r="N12" s="22">
         <v>18</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="22">
         <v>18</v>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="22">
         <v>17</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="22">
         <v>19</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="22">
         <v>17</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="22">
         <v>17</v>
       </c>
-      <c r="T12" s="26">
+      <c r="T12" s="22">
         <v>16</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="22">
         <v>18</v>
       </c>
       <c r="V12">
@@ -3686,6 +3769,30 @@
       </c>
       <c r="K13" t="s">
         <v>4</v>
+      </c>
+      <c r="N13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" s="36" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -3715,7 +3822,7 @@
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="13">
         <v>3</v>
       </c>
       <c r="C18" s="5">
@@ -3778,28 +3885,28 @@
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="30">
-        <v>1</v>
-      </c>
-      <c r="D19" s="30">
-        <v>0</v>
-      </c>
-      <c r="E19" s="30">
-        <v>0</v>
-      </c>
-      <c r="F19" s="30">
-        <v>0</v>
-      </c>
-      <c r="G19" s="30">
-        <v>0</v>
-      </c>
-      <c r="H19" s="30">
-        <v>0</v>
-      </c>
-      <c r="I19" s="30">
-        <v>0</v>
-      </c>
-      <c r="J19" s="30">
+      <c r="C19" s="26">
+        <v>1</v>
+      </c>
+      <c r="D19" s="26">
+        <v>0</v>
+      </c>
+      <c r="E19" s="26">
+        <v>0</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0</v>
+      </c>
+      <c r="H19" s="26">
+        <v>0</v>
+      </c>
+      <c r="I19" s="26">
+        <v>0</v>
+      </c>
+      <c r="J19" s="26">
         <v>2</v>
       </c>
       <c r="K19" s="1">
@@ -3812,28 +3919,28 @@
       <c r="N19" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="28">
+      <c r="O19" s="24">
         <v>8</v>
       </c>
-      <c r="P19" s="28">
+      <c r="P19" s="24">
         <v>11</v>
       </c>
-      <c r="Q19" s="28">
+      <c r="Q19" s="24">
         <v>8</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R19" s="24">
         <v>7</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S19" s="24">
         <v>15</v>
       </c>
-      <c r="T19" s="28">
+      <c r="T19" s="24">
         <v>14</v>
       </c>
-      <c r="U19" s="28">
+      <c r="U19" s="24">
         <v>11</v>
       </c>
-      <c r="V19" s="28">
+      <c r="V19" s="24">
         <v>14</v>
       </c>
       <c r="W19">
@@ -3852,28 +3959,28 @@
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" s="30">
-        <v>3</v>
-      </c>
-      <c r="D20" s="30">
-        <v>1</v>
-      </c>
-      <c r="E20" s="30">
-        <v>2</v>
-      </c>
-      <c r="F20" s="30">
-        <v>1</v>
-      </c>
-      <c r="G20" s="30">
-        <v>1</v>
-      </c>
-      <c r="H20" s="30">
-        <v>1</v>
-      </c>
-      <c r="I20" s="30">
-        <v>1</v>
-      </c>
-      <c r="J20" s="30">
+      <c r="C20" s="26">
+        <v>3</v>
+      </c>
+      <c r="D20" s="26">
+        <v>1</v>
+      </c>
+      <c r="E20" s="26">
+        <v>2</v>
+      </c>
+      <c r="F20" s="26">
+        <v>1</v>
+      </c>
+      <c r="G20" s="26">
+        <v>1</v>
+      </c>
+      <c r="H20" s="26">
+        <v>1</v>
+      </c>
+      <c r="I20" s="26">
+        <v>1</v>
+      </c>
+      <c r="J20" s="26">
         <v>3</v>
       </c>
       <c r="K20" s="1">
@@ -3886,28 +3993,28 @@
       <c r="N20" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="29">
+      <c r="O20" s="25">
         <v>17</v>
       </c>
-      <c r="P20" s="29">
+      <c r="P20" s="25">
         <v>19</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="Q20" s="25">
         <v>18</v>
       </c>
-      <c r="R20" s="29">
+      <c r="R20" s="25">
         <v>19</v>
       </c>
-      <c r="S20" s="29">
+      <c r="S20" s="25">
         <v>19</v>
       </c>
-      <c r="T20" s="29">
+      <c r="T20" s="25">
         <v>19</v>
       </c>
-      <c r="U20" s="29">
+      <c r="U20" s="25">
         <v>19</v>
       </c>
-      <c r="V20" s="29">
+      <c r="V20" s="25">
         <v>17</v>
       </c>
       <c r="W20">
@@ -3958,6 +4065,30 @@
       </c>
       <c r="L21" t="s">
         <v>4</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="U21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="V21" s="32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -4031,8 +4162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4344,28 +4475,28 @@
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="36">
-        <v>0</v>
-      </c>
-      <c r="C19" s="36">
-        <v>0</v>
-      </c>
-      <c r="D19" s="36">
-        <v>0</v>
-      </c>
-      <c r="E19" s="36">
-        <v>0</v>
-      </c>
-      <c r="F19" s="36">
-        <v>0</v>
-      </c>
-      <c r="G19" s="36">
-        <v>0</v>
-      </c>
-      <c r="H19" s="36">
-        <v>0</v>
-      </c>
-      <c r="I19" s="36">
+      <c r="B19" s="32">
+        <v>0</v>
+      </c>
+      <c r="C19" s="32">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>0</v>
+      </c>
+      <c r="H19" s="32">
+        <v>0</v>
+      </c>
+      <c r="I19" s="32">
         <v>0</v>
       </c>
       <c r="J19" s="1">
@@ -4378,28 +4509,28 @@
       <c r="M19" t="s">
         <v>10</v>
       </c>
-      <c r="N19" s="35">
+      <c r="N19" s="31">
         <v>14</v>
       </c>
-      <c r="O19" s="35">
+      <c r="O19" s="31">
         <v>17</v>
       </c>
-      <c r="P19" s="35">
+      <c r="P19" s="31">
         <v>17</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="31">
         <v>15</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="31">
         <v>17</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="31">
         <v>13</v>
       </c>
-      <c r="T19" s="35">
+      <c r="T19" s="31">
         <v>12</v>
       </c>
-      <c r="U19" s="35">
+      <c r="U19" s="31">
         <v>18</v>
       </c>
       <c r="V19">
@@ -4411,28 +4542,28 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="36">
-        <v>4</v>
-      </c>
-      <c r="C20" s="36">
-        <v>2</v>
-      </c>
-      <c r="D20" s="36">
-        <v>3</v>
-      </c>
-      <c r="E20" s="36">
-        <v>1</v>
-      </c>
-      <c r="F20" s="36">
-        <v>2</v>
-      </c>
-      <c r="G20" s="36">
-        <v>4</v>
-      </c>
-      <c r="H20" s="36">
-        <v>2</v>
-      </c>
-      <c r="I20" s="36">
+      <c r="B20" s="32">
+        <v>4</v>
+      </c>
+      <c r="C20" s="32">
+        <v>2</v>
+      </c>
+      <c r="D20" s="32">
+        <v>3</v>
+      </c>
+      <c r="E20" s="32">
+        <v>1</v>
+      </c>
+      <c r="F20" s="32">
+        <v>2</v>
+      </c>
+      <c r="G20" s="32">
+        <v>4</v>
+      </c>
+      <c r="H20" s="32">
+        <v>2</v>
+      </c>
+      <c r="I20" s="32">
         <v>2</v>
       </c>
       <c r="J20" s="1">
@@ -4445,28 +4576,28 @@
       <c r="M20" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="31">
         <v>16</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="31">
         <v>18</v>
       </c>
-      <c r="P20" s="35">
+      <c r="P20" s="31">
         <v>17</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q20" s="31">
         <v>19</v>
       </c>
-      <c r="R20" s="35">
+      <c r="R20" s="31">
         <v>18</v>
       </c>
-      <c r="S20" s="35">
+      <c r="S20" s="31">
         <v>16</v>
       </c>
-      <c r="T20" s="35">
+      <c r="T20" s="31">
         <v>18</v>
       </c>
-      <c r="U20" s="35">
+      <c r="U20" s="31">
         <v>18</v>
       </c>
       <c r="V20">
@@ -4513,6 +4644,30 @@
       </c>
       <c r="K21" t="s">
         <v>4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="U21" s="32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Most recent update - 12-29-14
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BNBO" sheetId="1" r:id="rId1"/>
@@ -86,13 +86,13 @@
     <t>For 6 trials, Intent detected but EEG_GO, EMG_GO decisions were 0</t>
   </si>
   <si>
-    <t>waitng for Ted's reply</t>
-  </si>
-  <si>
     <t>BD</t>
   </si>
   <si>
     <t>TR</t>
+  </si>
+  <si>
+    <t>blocks 1,3,5 not used for calculating EEG-EMG latencies because of problem with data</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -674,6 +674,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -985,7 +989,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1185,13 +1189,13 @@
         <v>4</v>
       </c>
       <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
         <v>23</v>
-      </c>
-      <c r="M5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1434,25 +1438,25 @@
         <v>4</v>
       </c>
       <c r="L13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -1719,28 +1723,28 @@
         <v>4</v>
       </c>
       <c r="M21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U21" s="32"/>
     </row>
@@ -1808,7 +1812,7 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="N10" sqref="N10:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2492,8 +2496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,7 +2681,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="N8" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2690,6 +2702,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2735,7 +2751,7 @@
       <c r="P10" s="5">
         <v>3</v>
       </c>
-      <c r="Q10" s="33">
+      <c r="Q10" s="37">
         <v>5</v>
       </c>
       <c r="R10" s="5">
@@ -2948,9 +2964,7 @@
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="34" t="s">
-        <v>22</v>
-      </c>
+      <c r="Q13" s="34"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -3304,6 +3318,9 @@
       <c r="O29" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N8:Q9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3500,16 +3517,16 @@
         <v>4</v>
       </c>
       <c r="K5" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3771,28 +3788,28 @@
         <v>4</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P13" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R13" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S13" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T13" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U13" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -4067,28 +4084,28 @@
         <v>4</v>
       </c>
       <c r="O21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V21" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -4162,7 +4179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
@@ -4646,28 +4663,28 @@
         <v>4</v>
       </c>
       <c r="N21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="32" t="s">
+      <c r="S21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="32" t="s">
+      <c r="T21" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Q21" s="32" t="s">
+      <c r="U21" s="32" t="s">
         <v>23</v>
-      </c>
-      <c r="R21" t="s">
-        <v>24</v>
-      </c>
-      <c r="S21" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="T21" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="U21" s="32" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
calculating detection latencies, UD vs UT comparison during simulated closed-loop
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BNBO" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="LSGR" sheetId="3" r:id="rId3"/>
     <sheet name="PLSH" sheetId="4" r:id="rId4"/>
     <sheet name="JF" sheetId="5" r:id="rId5"/>
+    <sheet name="Data for online-offline trainin" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="52">
   <si>
     <t>Ses 3</t>
   </si>
@@ -93,6 +94,87 @@
   </si>
   <si>
     <t>blocks 1,3,5 not used for calculating EEG-EMG latencies because of problem with data</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Total trials per class used for model training</t>
+  </si>
+  <si>
+    <t>Initial trials per class after artifact rejection</t>
+  </si>
+  <si>
+    <t>Trials belonging to Day 1, used for model training</t>
+  </si>
+  <si>
+    <t>Detection Latency (SD)</t>
+  </si>
+  <si>
+    <t>Adaptive Window</t>
+  </si>
+  <si>
+    <t>Fixed Window</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Detection latency (mean) (sec.)</t>
+  </si>
+  <si>
+    <t>Optimal window length (sec.)</t>
+  </si>
+  <si>
+    <t>weighted mean and standard deviation</t>
+  </si>
+  <si>
+    <t>Number of Intent Detections (True Positives)</t>
+  </si>
+  <si>
+    <t>Trials used for training (Blockwise)</t>
+  </si>
+  <si>
+    <t>Latency during closed-loop control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day4 (BD) </t>
+  </si>
+  <si>
+    <t>Day 5(AT)</t>
+  </si>
+  <si>
+    <t>Day4(AT)</t>
+  </si>
+  <si>
+    <t>Day5(AT)</t>
+  </si>
+  <si>
+    <t>Day4(BD)</t>
+  </si>
+  <si>
+    <t>remove outliers</t>
+  </si>
+  <si>
+    <t>day 4 only</t>
+  </si>
+  <si>
+    <t>day 5 only</t>
   </si>
 </sst>
 </file>
@@ -625,7 +707,7 @@
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -677,7 +759,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -989,7 +1091,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1000,7 +1102,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,7 +1463,7 @@
       <c r="H12" s="14">
         <v>2</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="42">
         <f>SUM(B12:H12)</f>
         <v>19</v>
       </c>
@@ -1393,7 +1495,7 @@
       <c r="R12" s="15">
         <v>18</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="41">
         <f>SUM(L12:R12)</f>
         <v>121</v>
       </c>
@@ -1468,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1639,7 +1741,7 @@
       <c r="I20" s="17">
         <v>4</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="42">
         <f>SUM(B20:I20)</f>
         <v>25</v>
       </c>
@@ -1674,9 +1776,9 @@
       <c r="T20" s="16">
         <v>16</v>
       </c>
-      <c r="U20">
-        <f>SUM(N20:T20)</f>
-        <v>119</v>
+      <c r="U20" s="41">
+        <f>SUM(M20:T20)</f>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
@@ -1803,7 +1905,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1811,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10:U11"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2082,7 +2184,7 @@
       <c r="I12" s="32">
         <v>4</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="42">
         <f>SUM(B12:I12)</f>
         <v>22</v>
       </c>
@@ -2117,12 +2219,12 @@
       <c r="U12" s="32">
         <v>16</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="41">
         <f>SUM(N12:U12)</f>
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2178,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J14">
         <f>_xlfn.STDEV.S(B13:I13)</f>
         <v>0.44039574554985511</v>
@@ -2187,7 +2289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2329,7 +2431,7 @@
       <c r="H20" s="19">
         <v>4</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="42">
         <f>SUM(B20:H20)</f>
         <v>15</v>
       </c>
@@ -2355,7 +2457,7 @@
       <c r="R20" s="18">
         <v>16</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="41">
         <f>SUM(N20:R20)</f>
         <v>85</v>
       </c>
@@ -2496,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2682,12 +2784,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
     </row>
     <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -2702,10 +2804,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2873,7 +2975,7 @@
       <c r="J12" s="28">
         <v>4</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="42">
         <f>SUM(B12:J12)</f>
         <v>21</v>
       </c>
@@ -2907,7 +3009,7 @@
       <c r="U12" s="10">
         <v>16</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="41">
         <f>SUM(N12:U12)</f>
         <v>139</v>
       </c>
@@ -2979,7 +3081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3165,7 +3267,7 @@
       <c r="J20" s="30">
         <v>2</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="42">
         <f>SUM(B20:J20)</f>
         <v>22</v>
       </c>
@@ -3203,7 +3305,7 @@
       <c r="W20" s="29">
         <v>18</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="41">
         <f>SUM(O20:W20)</f>
         <v>158</v>
       </c>
@@ -3330,7 +3432,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3708,7 +3810,7 @@
       <c r="I12" s="23">
         <v>2</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="42">
         <f>SUM(B12:I12)</f>
         <v>20</v>
       </c>
@@ -3742,7 +3844,7 @@
       <c r="U12" s="22">
         <v>18</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="41">
         <f>SUM(N12:U12)</f>
         <v>140</v>
       </c>
@@ -3821,7 +3923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -4000,9 +4102,9 @@
       <c r="J20" s="26">
         <v>3</v>
       </c>
-      <c r="K20" s="1">
-        <f>SUM(B20:J20)</f>
-        <v>16</v>
+      <c r="K20" s="42">
+        <f>SUM(C20:J20)</f>
+        <v>13</v>
       </c>
       <c r="L20" s="9">
         <v>4</v>
@@ -4034,7 +4136,7 @@
       <c r="V20" s="25">
         <v>17</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="41">
         <f>SUM(O20:V20)</f>
         <v>147</v>
       </c>
@@ -4078,7 +4180,7 @@
       </c>
       <c r="K21" s="1">
         <f>K19/K20</f>
-        <v>0.1875</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
@@ -4384,7 +4486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>B11/B12</f>
         <v>0.33333333333333331</v>
@@ -4409,7 +4511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F14">
         <f>_xlfn.STDEV.S(B13:E13)</f>
         <v>0.47140452079103168</v>
@@ -4418,7 +4520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -4741,4 +4843,808 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="38"/>
+    <col min="3" max="3" width="19.77734375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="38" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="38" customWidth="1"/>
+    <col min="6" max="9" width="16.33203125" style="38" customWidth="1"/>
+    <col min="10" max="11" width="18.33203125" style="38" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="38" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" style="38" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="F1" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="O1" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="39" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="43">
+        <v>1</v>
+      </c>
+      <c r="P2" s="43">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="43">
+        <v>3</v>
+      </c>
+      <c r="R2" s="43">
+        <v>4</v>
+      </c>
+      <c r="S2" s="43">
+        <v>5</v>
+      </c>
+      <c r="T2" s="43">
+        <v>6</v>
+      </c>
+      <c r="U2" s="43">
+        <v>7</v>
+      </c>
+      <c r="V2" s="43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="40">
+        <v>134</v>
+      </c>
+      <c r="D3" s="40">
+        <v>101</v>
+      </c>
+      <c r="E3" s="40">
+        <v>62</v>
+      </c>
+      <c r="F3" s="40">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="40">
+        <v>84</v>
+      </c>
+      <c r="H3" s="40">
+        <v>-0.78100000000000003</v>
+      </c>
+      <c r="I3" s="40">
+        <v>0.66510000000000002</v>
+      </c>
+      <c r="J3" s="38">
+        <v>1</v>
+      </c>
+      <c r="K3" s="38">
+        <v>132</v>
+      </c>
+      <c r="L3" s="38">
+        <v>-0.91969999999999996</v>
+      </c>
+      <c r="M3" s="38">
+        <v>0.58230000000000004</v>
+      </c>
+      <c r="O3" s="38">
+        <v>18</v>
+      </c>
+      <c r="P3" s="38">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="38">
+        <v>14</v>
+      </c>
+      <c r="R3" s="38">
+        <v>14</v>
+      </c>
+      <c r="S3" s="38">
+        <v>11</v>
+      </c>
+      <c r="T3" s="38">
+        <v>12</v>
+      </c>
+      <c r="U3" s="38">
+        <v>16</v>
+      </c>
+      <c r="V3" s="38">
+        <v>0</v>
+      </c>
+      <c r="W3" s="38">
+        <f t="shared" ref="W3:W8" si="0">SUM(O3:V3)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="40">
+        <v>154</v>
+      </c>
+      <c r="D4" s="40">
+        <v>107</v>
+      </c>
+      <c r="E4" s="40">
+        <v>56</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="G4" s="40">
+        <v>89</v>
+      </c>
+      <c r="H4" s="40">
+        <v>-0.86629999999999996</v>
+      </c>
+      <c r="I4" s="40">
+        <v>0.55059999999999998</v>
+      </c>
+      <c r="J4" s="38">
+        <v>1</v>
+      </c>
+      <c r="K4" s="38">
+        <v>153</v>
+      </c>
+      <c r="L4" s="38">
+        <v>-0.95750000000000002</v>
+      </c>
+      <c r="M4" s="38">
+        <v>0.56259999999999999</v>
+      </c>
+      <c r="O4" s="38">
+        <v>15</v>
+      </c>
+      <c r="P4" s="38">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="38">
+        <v>12</v>
+      </c>
+      <c r="R4" s="38">
+        <v>16</v>
+      </c>
+      <c r="S4" s="38">
+        <v>16</v>
+      </c>
+      <c r="T4" s="38">
+        <v>11</v>
+      </c>
+      <c r="U4" s="38">
+        <v>11</v>
+      </c>
+      <c r="V4" s="38">
+        <v>13</v>
+      </c>
+      <c r="W4" s="38">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="40">
+        <v>160</v>
+      </c>
+      <c r="D5" s="40">
+        <v>116</v>
+      </c>
+      <c r="E5" s="40">
+        <v>56</v>
+      </c>
+      <c r="F5" s="40">
+        <v>0.85</v>
+      </c>
+      <c r="G5" s="40">
+        <v>79</v>
+      </c>
+      <c r="H5" s="40">
+        <v>-0.68230000000000002</v>
+      </c>
+      <c r="I5" s="40">
+        <v>0.66169999999999995</v>
+      </c>
+      <c r="J5" s="38">
+        <v>0.95</v>
+      </c>
+      <c r="K5" s="38">
+        <v>149</v>
+      </c>
+      <c r="L5" s="38">
+        <v>-0.91279999999999994</v>
+      </c>
+      <c r="M5" s="38">
+        <v>0.64929999999999999</v>
+      </c>
+      <c r="O5" s="38">
+        <v>17</v>
+      </c>
+      <c r="P5" s="38">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="38">
+        <v>13</v>
+      </c>
+      <c r="R5" s="38">
+        <v>10</v>
+      </c>
+      <c r="S5" s="38">
+        <v>15</v>
+      </c>
+      <c r="T5" s="38">
+        <v>15</v>
+      </c>
+      <c r="U5" s="38">
+        <v>13</v>
+      </c>
+      <c r="V5" s="38">
+        <v>17</v>
+      </c>
+      <c r="W5" s="38">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="40">
+        <v>157</v>
+      </c>
+      <c r="D6" s="40">
+        <v>105</v>
+      </c>
+      <c r="E6" s="40">
+        <v>57</v>
+      </c>
+      <c r="F6" s="40">
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="40">
+        <v>74</v>
+      </c>
+      <c r="H6" s="40">
+        <v>-0.877</v>
+      </c>
+      <c r="I6" s="40">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="J6" s="38">
+        <v>0.95</v>
+      </c>
+      <c r="K6" s="38">
+        <v>156</v>
+      </c>
+      <c r="L6" s="38">
+        <v>-0.88560000000000005</v>
+      </c>
+      <c r="M6" s="38">
+        <v>0.66910000000000003</v>
+      </c>
+      <c r="O6" s="38">
+        <v>17</v>
+      </c>
+      <c r="P6" s="38">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="38">
+        <v>13</v>
+      </c>
+      <c r="R6" s="38">
+        <v>13</v>
+      </c>
+      <c r="S6" s="38">
+        <v>9</v>
+      </c>
+      <c r="T6" s="38">
+        <v>12</v>
+      </c>
+      <c r="U6" s="38">
+        <v>12</v>
+      </c>
+      <c r="V6" s="38">
+        <v>15</v>
+      </c>
+      <c r="W6" s="38">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="40">
+        <v>160</v>
+      </c>
+      <c r="D7" s="40">
+        <v>131</v>
+      </c>
+      <c r="E7" s="40">
+        <v>60</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0.65</v>
+      </c>
+      <c r="G7" s="40">
+        <v>124</v>
+      </c>
+      <c r="H7" s="40">
+        <v>-0.7339</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0.73880000000000001</v>
+      </c>
+      <c r="J7" s="38">
+        <v>1</v>
+      </c>
+      <c r="K7" s="38">
+        <v>159</v>
+      </c>
+      <c r="L7" s="38">
+        <v>-1.1295999999999999</v>
+      </c>
+      <c r="M7" s="38">
+        <v>0.43290000000000001</v>
+      </c>
+      <c r="O7" s="38">
+        <v>14</v>
+      </c>
+      <c r="P7" s="38">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>16</v>
+      </c>
+      <c r="R7" s="38">
+        <v>16</v>
+      </c>
+      <c r="S7" s="38">
+        <v>18</v>
+      </c>
+      <c r="T7" s="38">
+        <v>18</v>
+      </c>
+      <c r="U7" s="38">
+        <v>18</v>
+      </c>
+      <c r="V7" s="38">
+        <v>17</v>
+      </c>
+      <c r="W7" s="38">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="40">
+        <v>160</v>
+      </c>
+      <c r="D8" s="40">
+        <v>140</v>
+      </c>
+      <c r="E8" s="40">
+        <v>70</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="G8" s="40">
+        <v>130</v>
+      </c>
+      <c r="H8" s="40">
+        <v>-0.38690000000000002</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0.63570000000000004</v>
+      </c>
+      <c r="J8" s="38">
+        <v>0.85</v>
+      </c>
+      <c r="K8" s="38">
+        <v>155</v>
+      </c>
+      <c r="L8" s="38">
+        <v>-0.87480000000000002</v>
+      </c>
+      <c r="M8" s="38">
+        <v>0.65559999999999996</v>
+      </c>
+      <c r="O8" s="38">
+        <v>16</v>
+      </c>
+      <c r="P8" s="38">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="38">
+        <v>17</v>
+      </c>
+      <c r="R8" s="38">
+        <v>19</v>
+      </c>
+      <c r="S8" s="38">
+        <v>18</v>
+      </c>
+      <c r="T8" s="38">
+        <v>15</v>
+      </c>
+      <c r="U8" s="38">
+        <v>18</v>
+      </c>
+      <c r="V8" s="38">
+        <v>19</v>
+      </c>
+      <c r="W8" s="38">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C9" s="38">
+        <f>SUM(C3:C8)</f>
+        <v>925</v>
+      </c>
+      <c r="D9" s="38">
+        <f>SUM(D3:D8)</f>
+        <v>700</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="45"/>
+      <c r="H9" s="40">
+        <v>-0.69450000000000001</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0.19420000000000001</v>
+      </c>
+      <c r="K9" s="40">
+        <v>-0.94830000000000003</v>
+      </c>
+      <c r="L9" s="40">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="O9" s="38">
+        <f t="shared" ref="O9:U9" si="1">AVERAGE(O3:O8)</f>
+        <v>16.166666666666668</v>
+      </c>
+      <c r="P9" s="38">
+        <f t="shared" si="1"/>
+        <v>15.166666666666666</v>
+      </c>
+      <c r="Q9" s="38">
+        <f t="shared" si="1"/>
+        <v>14.166666666666666</v>
+      </c>
+      <c r="R9" s="38">
+        <f t="shared" si="1"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="S9" s="38">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="T9" s="38">
+        <f t="shared" si="1"/>
+        <v>13.833333333333334</v>
+      </c>
+      <c r="U9" s="38">
+        <f t="shared" si="1"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="V9" s="38">
+        <f>AVERAGE(V4:V8)</f>
+        <v>16.2</v>
+      </c>
+      <c r="W9" s="38">
+        <f>AVERAGE(W3:W8)</f>
+        <v>116.66666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="F11" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+    </row>
+    <row r="12" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40">
+        <v>69</v>
+      </c>
+      <c r="H13" s="40">
+        <v>-0.49680000000000002</v>
+      </c>
+      <c r="I13" s="40">
+        <v>0.42730000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B14" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40">
+        <v>106</v>
+      </c>
+      <c r="H14" s="40">
+        <v>-0.45650000000000002</v>
+      </c>
+      <c r="I14" s="40">
+        <v>0.40079999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40">
+        <v>108</v>
+      </c>
+      <c r="H15" s="40">
+        <v>-0.6825</v>
+      </c>
+      <c r="I15" s="40">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B16" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40">
+        <v>88</v>
+      </c>
+      <c r="H16" s="40">
+        <v>-0.48370000000000002</v>
+      </c>
+      <c r="I16" s="40">
+        <v>0.56179999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40">
+        <v>76</v>
+      </c>
+      <c r="H17" s="40">
+        <v>-0.34589999999999999</v>
+      </c>
+      <c r="I17" s="40">
+        <v>0.38969999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40">
+        <v>57</v>
+      </c>
+      <c r="H18" s="40">
+        <v>-0.60870000000000002</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0.3206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40">
+        <v>73</v>
+      </c>
+      <c r="H19" s="40">
+        <v>-0.30680000000000002</v>
+      </c>
+      <c r="I19" s="40">
+        <v>0.50470000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40">
+        <v>107</v>
+      </c>
+      <c r="H20" s="40">
+        <v>0.29509999999999997</v>
+      </c>
+      <c r="I20" s="40">
+        <v>0.89939999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="45"/>
+      <c r="H21" s="40">
+        <v>-0.36659999999999998</v>
+      </c>
+      <c r="I21" s="40">
+        <v>0.32829999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G22" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="38">
+        <v>-0.48060000000000003</v>
+      </c>
+      <c r="I22" s="38">
+        <v>0.18090000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G23" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="38">
+        <v>-0.26279999999999998</v>
+      </c>
+      <c r="I23" s="38">
+        <v>0.42449999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="F11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files to analyze clinical study data
</commit_message>
<xml_diff>
--- a/Analyzing Catch Trials_Nikunj.xlsx
+++ b/Analyzing Catch Trials_Nikunj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="6072" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16176" windowHeight="8412" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BNBO" sheetId="1" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,8 +1709,8 @@
         <v>106</v>
       </c>
       <c r="V19">
-        <f>102/119</f>
-        <v>0.8571428571428571</v>
+        <f>106/135</f>
+        <v>0.78518518518518521</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
@@ -3429,10 +3429,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3440,7 +3440,7 @@
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3450,7 +3450,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>0.52112676056338025</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="G6" t="e">
         <f>_xlfn.STDEV.S(B5:F5)</f>
         <v>#DIV/0!</v>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3777,12 +3777,8 @@
         <f>SUM(N11:U11)</f>
         <v>113</v>
       </c>
-      <c r="W11">
-        <f>109/140</f>
-        <v>0.77857142857142858</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3849,7 +3845,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>B11/B12</f>
         <v>0</v>
@@ -3914,7 +3910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="J14">
         <f>_xlfn.STDEV.S(B13:I13)</f>
         <v>0</v>
@@ -3923,7 +3919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -3937,7 +3933,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3997,7 +3993,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4066,12 +4062,8 @@
         <f>SUM(O19:V19)</f>
         <v>88</v>
       </c>
-      <c r="X19">
-        <f>85/164</f>
-        <v>0.51829268292682928</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -4141,7 +4133,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" ref="B21:J21" si="2">B19/B20</f>
         <v>0</v>
@@ -4210,7 +4202,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="K22">
         <f>_xlfn.STDEV.S(B21:J21)*100</f>
         <v>23.570226039551585</v>
@@ -4222,10 +4214,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>15</v>
       </c>
@@ -4234,7 +4226,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>16</v>
       </c>
@@ -4247,10 +4239,10 @@
       </c>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>17</v>
       </c>
@@ -4259,7 +4251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>18</v>
       </c>
@@ -4849,7 +4841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>

</xml_diff>